<commit_message>
ignoring csv and xlsx
</commit_message>
<xml_diff>
--- a/optimizer_results.xlsx
+++ b/optimizer_results.xlsx
@@ -16,9 +16,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="0.0000"/>
-  </numFmts>
+  <numFmts count="0"/>
   <fonts count="2">
     <font>
       <name val="Calibri"/>
@@ -68,7 +66,7 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="right" vertical="center"/>
     </xf>
   </cellXfs>
@@ -436,7 +434,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E18"/>
+  <dimension ref="A1:E8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -444,7 +442,7 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
-    <col width="83" customWidth="1" min="1" max="1"/>
+    <col width="18" customWidth="1" min="1" max="1"/>
     <col width="20" customWidth="1" min="2" max="2"/>
     <col width="20" customWidth="1" min="3" max="3"/>
     <col width="20" customWidth="1" min="4" max="4"/>
@@ -481,55 +479,55 @@
     <row r="2">
       <c r="A2" s="2" t="inlineStr">
         <is>
-          <t>&lt;keras.optimizers.optimizer_v2.gradient_descent.SGD object at 0x000002088C929850&gt;</t>
+          <t>gradient_descent</t>
         </is>
       </c>
       <c r="B2" s="2" t="n">
-        <v>0.5397713780403137</v>
+        <v>0.5390639901161194</v>
       </c>
       <c r="C2" s="2" t="n">
-        <v>0.7372564077377319</v>
+        <v>0.7379853129386902</v>
       </c>
       <c r="D2" s="2" t="n">
-        <v>0.5605036616325378</v>
+        <v>0.5547692179679871</v>
       </c>
       <c r="E2" s="2" t="n">
-        <v>0.7199222445487976</v>
+        <v>0.7259474992752075</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="2" t="inlineStr">
         <is>
-          <t>&lt;keras.optimizers.optimizer_v2.adam.Adam object at 0x000002088C9297F0&gt;</t>
+          <t>adam</t>
         </is>
       </c>
       <c r="B3" s="2" t="n">
-        <v>0.5400733947753906</v>
+        <v>0.5379234552383423</v>
       </c>
       <c r="C3" s="2" t="n">
-        <v>0.7385198473930359</v>
+        <v>0.7377909421920776</v>
       </c>
       <c r="D3" s="2" t="n">
-        <v>0.5634080767631531</v>
+        <v>0.5631925463676453</v>
       </c>
       <c r="E3" s="2" t="n">
-        <v>0.7259474992752075</v>
+        <v>0.7230320572853088</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="2" t="inlineStr">
         <is>
-          <t>&lt;keras.optimizers.optimizer_v2.rmsprop.RMSprop object at 0x000002088C929040&gt;</t>
+          <t>rmsprop</t>
         </is>
       </c>
       <c r="B4" s="2" t="n">
-        <v>0.5425463318824768</v>
+        <v>0.5421916246414185</v>
       </c>
       <c r="C4" s="2" t="n">
-        <v>0.7384712696075439</v>
+        <v>0.7386170625686646</v>
       </c>
       <c r="D4" s="2" t="n">
-        <v>0.5641368627548218</v>
+        <v>0.5695213079452515</v>
       </c>
       <c r="E4" s="2" t="n">
         <v>0.7255588173866272</v>
@@ -538,267 +536,77 @@
     <row r="5">
       <c r="A5" s="2" t="inlineStr">
         <is>
-          <t>&lt;keras.optimizers.optimizer_v2.adagrad.Adagrad object at 0x000002088C929910&gt;</t>
+          <t>adagrad</t>
         </is>
       </c>
       <c r="B5" s="2" t="n">
-        <v>0.5331329107284546</v>
+        <v>0.5334345102310181</v>
       </c>
       <c r="C5" s="2" t="n">
-        <v>0.742261528968811</v>
+        <v>0.7420185804367065</v>
       </c>
       <c r="D5" s="2" t="n">
-        <v>0.5570952892303467</v>
+        <v>0.5591048002243042</v>
       </c>
       <c r="E5" s="2" t="n">
-        <v>0.7234207987785339</v>
+        <v>0.7243925929069519</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="2" t="inlineStr">
         <is>
-          <t>&lt;keras.optimizers.optimizer_v2.adadelta.Adadelta object at 0x000002088C929490&gt;</t>
+          <t>adadelta</t>
         </is>
       </c>
       <c r="B6" s="2" t="n">
-        <v>0.5330867171287537</v>
+        <v>0.5334943532943726</v>
       </c>
       <c r="C6" s="2" t="n">
-        <v>0.742261528968811</v>
+        <v>0.7421157360076904</v>
       </c>
       <c r="D6" s="2" t="n">
-        <v>0.5571774840354919</v>
+        <v>0.5591701865196228</v>
       </c>
       <c r="E6" s="2" t="n">
-        <v>0.7234207987785339</v>
+        <v>0.7243925929069519</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="2" t="inlineStr">
         <is>
-          <t>&lt;keras.optimizers.optimizer_v2.adamax.Adamax object at 0x000002088C9291C0&gt;</t>
+          <t>adamax</t>
         </is>
       </c>
       <c r="B7" s="2" t="n">
-        <v>0.5328463315963745</v>
+        <v>0.5328094363212585</v>
       </c>
       <c r="C7" s="2" t="n">
-        <v>0.7416298389434814</v>
+        <v>0.7425044775009155</v>
       </c>
       <c r="D7" s="2" t="n">
-        <v>0.5579150915145874</v>
+        <v>0.559444785118103</v>
       </c>
       <c r="E7" s="2" t="n">
-        <v>0.722449004650116</v>
+        <v>0.724781334400177</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="2" t="inlineStr">
         <is>
-          <t>&lt;keras.optimizers.optimizer_v2.nadam.Nadam object at 0x000002088C9293D0&gt;</t>
+          <t>nadam</t>
         </is>
       </c>
       <c r="B8" s="2" t="n">
-        <v>0.5358962416648865</v>
+        <v>0.5347521305084229</v>
       </c>
       <c r="C8" s="2" t="n">
-        <v>0.7417269945144653</v>
+        <v>0.7408522963523865</v>
       </c>
       <c r="D8" s="2" t="n">
-        <v>0.5600679516792297</v>
+        <v>0.5613396763801575</v>
       </c>
       <c r="E8" s="2" t="n">
-        <v>0.7208940982818604</v>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" s="2" t="inlineStr">
-        <is>
-          <t>gradient_descent</t>
-        </is>
-      </c>
-      <c r="B9" s="2" t="n">
-        <v>0.5327004194259644</v>
-      </c>
-      <c r="C9" s="2" t="n">
-        <v>0.7430390119552612</v>
-      </c>
-      <c r="D9" s="2" t="n">
-        <v>0.5591812133789062</v>
-      </c>
-      <c r="E9" s="2" t="n">
-        <v>0.7208940982818604</v>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" s="2" t="inlineStr">
-        <is>
-          <t>adam</t>
-        </is>
-      </c>
-      <c r="B10" s="2" t="n">
-        <v>0.5368513464927673</v>
-      </c>
-      <c r="C10" s="2" t="n">
-        <v>0.7406579256057739</v>
-      </c>
-      <c r="D10" s="2" t="n">
-        <v>0.5639895796775818</v>
-      </c>
-      <c r="E10" s="2" t="n">
-        <v>0.7263362407684326</v>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" s="2" t="inlineStr">
-        <is>
-          <t>rmsprop</t>
-        </is>
-      </c>
-      <c r="B11" s="2" t="n">
-        <v>0.5395587086677551</v>
-      </c>
-      <c r="C11" s="2" t="n">
-        <v>0.7395402789115906</v>
-      </c>
-      <c r="D11" s="2" t="n">
-        <v>0.5694922208786011</v>
-      </c>
-      <c r="E11" s="2" t="n">
-        <v>0.7251700758934021</v>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12" s="2" t="inlineStr">
-        <is>
-          <t>gradient_descent</t>
-        </is>
-      </c>
-      <c r="B12" s="2" t="n">
-        <v>0.5335593819618225</v>
-      </c>
-      <c r="C12" s="2" t="n">
-        <v>0.7423587441444397</v>
-      </c>
-      <c r="D12" s="2" t="n">
-        <v>0.5604321360588074</v>
-      </c>
-      <c r="E12" s="2" t="n">
         <v>0.7261418700218201</v>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13" s="2" t="inlineStr">
-        <is>
-          <t>adam</t>
-        </is>
-      </c>
-      <c r="B13" s="2" t="n">
-        <v>0.5405787825584412</v>
-      </c>
-      <c r="C13" s="2" t="n">
-        <v>0.7394917011260986</v>
-      </c>
-      <c r="D13" s="2" t="n">
-        <v>0.5627157688140869</v>
-      </c>
-      <c r="E13" s="2" t="n">
-        <v>0.7232264280319214</v>
-      </c>
-    </row>
-    <row r="14">
-      <c r="A14" s="2" t="inlineStr">
-        <is>
-          <t>rmsprop</t>
-        </is>
-      </c>
-      <c r="B14" s="2" t="n">
-        <v>0.5521032810211182</v>
-      </c>
-      <c r="C14" s="2" t="n">
-        <v>0.7376937866210938</v>
-      </c>
-      <c r="D14" s="2" t="n">
-        <v>0.5880184769630432</v>
-      </c>
-      <c r="E14" s="2" t="n">
-        <v>0.7249757051467896</v>
-      </c>
-    </row>
-    <row r="15">
-      <c r="A15" s="2" t="inlineStr">
-        <is>
-          <t>adagrad</t>
-        </is>
-      </c>
-      <c r="B15" s="2" t="n">
-        <v>0.5370584726333618</v>
-      </c>
-      <c r="C15" s="2" t="n">
-        <v>0.7411924600601196</v>
-      </c>
-      <c r="D15" s="2" t="n">
-        <v>0.5687416791915894</v>
-      </c>
-      <c r="E15" s="2" t="n">
-        <v>0.7249757051467896</v>
-      </c>
-    </row>
-    <row r="16">
-      <c r="A16" s="2" t="inlineStr">
-        <is>
-          <t>adadelta</t>
-        </is>
-      </c>
-      <c r="B16" s="2" t="n">
-        <v>0.5368443131446838</v>
-      </c>
-      <c r="C16" s="2" t="n">
-        <v>0.7411924600601196</v>
-      </c>
-      <c r="D16" s="2" t="n">
-        <v>0.5688140988349915</v>
-      </c>
-      <c r="E16" s="2" t="n">
-        <v>0.7249757051467896</v>
-      </c>
-    </row>
-    <row r="17">
-      <c r="A17" s="2" t="inlineStr">
-        <is>
-          <t>adamax</t>
-        </is>
-      </c>
-      <c r="B17" s="2" t="n">
-        <v>0.5333966016769409</v>
-      </c>
-      <c r="C17" s="2" t="n">
-        <v>0.7422129511833191</v>
-      </c>
-      <c r="D17" s="2" t="n">
-        <v>0.5614777803421021</v>
-      </c>
-      <c r="E17" s="2" t="n">
-        <v>0.7267249822616577</v>
-      </c>
-    </row>
-    <row r="18">
-      <c r="A18" s="2" t="inlineStr">
-        <is>
-          <t>nadam</t>
-        </is>
-      </c>
-      <c r="B18" s="2" t="n">
-        <v>0.5394867658615112</v>
-      </c>
-      <c r="C18" s="2" t="n">
-        <v>0.7404149770736694</v>
-      </c>
-      <c r="D18" s="2" t="n">
-        <v>0.5701760649681091</v>
-      </c>
-      <c r="E18" s="2" t="n">
-        <v>0.7271137237548828</v>
       </c>
     </row>
   </sheetData>

</xml_diff>